<commit_message>
Added new versioning to pipeline template file, updated template
</commit_message>
<xml_diff>
--- a/templates/template-4c-pipeline.xlsx
+++ b/templates/template-4c-pipeline.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\dsday_scratch\fourfold\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\dsday_scratch\fourfold\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Options" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Normalization" sheetId="2" r:id="rId3"/>
     <sheet name="Smoothing" sheetId="3" r:id="rId4"/>
     <sheet name="Plots" sheetId="4" r:id="rId5"/>
+    <sheet name="Quantification" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>All</t>
   </si>
@@ -119,11 +120,14 @@
   <si>
     <t>This is an example -- this will not be run unless you remove the comment character at the beginning</t>
   </si>
+  <si>
+    <t>Template Version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,20 +477,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.15625" customWidth="1"/>
+    <col min="3" max="3" width="9.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -497,7 +501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -505,7 +509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -513,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -521,7 +525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -529,12 +533,20 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -551,13 +563,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -565,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -586,13 +598,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -600,7 +612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -622,15 +634,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -644,7 +656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -667,23 +679,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="91.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="91.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -709,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -738,4 +750,31 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15.47265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>